<commit_message>
New Era fix name
</commit_message>
<xml_diff>
--- a/Excel/New Era/2022.06.15/16.06.2022 NEW ERA — загрузка.xlsx
+++ b/Excel/New Era/2022.06.15/16.06.2022 NEW ERA — загрузка.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\New Era\2022.06.15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5412ED7-2DD4-42E1-82B8-716F865DA940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47120FB5-1289-4931-A5C1-25DC2EAA2251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3E57CB4D-01F2-45F7-8F67-AA1D52A73E62}"/>
   </bookViews>
@@ -1358,9 +1358,6 @@
     <t>Шапка NEW ERA арт. 60102591 Los Angeles Clippers (серый)</t>
   </si>
   <si>
-    <t>Шапка NEW ERA арт. 60102591 Los Angeles Clippers (серый) {otc}</t>
-  </si>
-  <si>
     <t>96-089-80-00</t>
   </si>
   <si>
@@ -2088,6 +2085,9 @@
   </si>
   <si>
     <t>ГТД</t>
+  </si>
+  <si>
+    <t>Шапка NEW ERA арт. 60102591 Los Angeles Clippers (серый) {otc}</t>
   </si>
 </sst>
 </file>
@@ -2618,9 +2618,9 @@
   </sheetPr>
   <dimension ref="A1:Y127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q68" sqref="Q68"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W88" sqref="W88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,7 +2700,7 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
@@ -8742,18 +8742,18 @@
         <v>429</v>
       </c>
       <c r="W82" t="s">
-        <v>430</v>
+        <v>673</v>
       </c>
       <c r="X82" t="s">
         <v>63</v>
       </c>
       <c r="Y82" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B83">
         <v>12881461</v>
@@ -8792,7 +8792,7 @@
       <c r="N83"/>
       <c r="O83"/>
       <c r="P83" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Q83">
         <v>1978.48</v>
@@ -8810,21 +8810,21 @@
         <v>38</v>
       </c>
       <c r="V83" t="s">
+        <v>433</v>
+      </c>
+      <c r="W83" t="s">
         <v>434</v>
-      </c>
-      <c r="W83" t="s">
-        <v>435</v>
       </c>
       <c r="X83" t="s">
         <v>48</v>
       </c>
       <c r="Y83" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B84">
         <v>12573358</v>
@@ -8865,7 +8865,7 @@
       <c r="N84"/>
       <c r="O84"/>
       <c r="P84" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Q84">
         <v>1978.48</v>
@@ -8883,24 +8883,24 @@
         <v>38</v>
       </c>
       <c r="V84" t="s">
+        <v>438</v>
+      </c>
+      <c r="W84" t="s">
         <v>439</v>
-      </c>
-      <c r="W84" t="s">
-        <v>440</v>
       </c>
       <c r="X84" t="s">
         <v>168</v>
       </c>
       <c r="Y84" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>441</v>
+      </c>
+      <c r="B85" t="s">
         <v>442</v>
-      </c>
-      <c r="B85" t="s">
-        <v>443</v>
       </c>
       <c r="C85" t="s">
         <v>45</v>
@@ -8918,7 +8918,7 @@
         <v>29</v>
       </c>
       <c r="H85" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I85" t="s">
         <v>314</v>
@@ -8940,7 +8940,7 @@
         <v>60</v>
       </c>
       <c r="P85" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Q85">
         <v>1722.48</v>
@@ -8958,24 +8958,24 @@
         <v>38</v>
       </c>
       <c r="V85" t="s">
+        <v>445</v>
+      </c>
+      <c r="W85" t="s">
         <v>446</v>
-      </c>
-      <c r="W85" t="s">
-        <v>447</v>
       </c>
       <c r="X85" t="s">
         <v>314</v>
       </c>
       <c r="Y85" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>448</v>
+      </c>
+      <c r="B86" t="s">
         <v>449</v>
-      </c>
-      <c r="B86" t="s">
-        <v>450</v>
       </c>
       <c r="C86" t="s">
         <v>45</v>
@@ -8993,7 +8993,7 @@
         <v>29</v>
       </c>
       <c r="H86" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I86" t="s">
         <v>63</v>
@@ -9035,21 +9035,21 @@
         <v>38</v>
       </c>
       <c r="V86" t="s">
+        <v>451</v>
+      </c>
+      <c r="W86" t="s">
         <v>452</v>
-      </c>
-      <c r="W86" t="s">
-        <v>453</v>
       </c>
       <c r="X86" t="s">
         <v>63</v>
       </c>
       <c r="Y86" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B87">
         <v>12505780</v>
@@ -9070,10 +9070,10 @@
         <v>29</v>
       </c>
       <c r="H87" t="s">
+        <v>455</v>
+      </c>
+      <c r="I87" t="s">
         <v>456</v>
-      </c>
-      <c r="I87" t="s">
-        <v>457</v>
       </c>
       <c r="J87" t="s">
         <v>197</v>
@@ -9106,21 +9106,21 @@
         <v>38</v>
       </c>
       <c r="V87" t="s">
+        <v>457</v>
+      </c>
+      <c r="W87" t="s">
         <v>458</v>
       </c>
-      <c r="W87" t="s">
+      <c r="X87" t="s">
+        <v>456</v>
+      </c>
+      <c r="Y87" t="s">
         <v>459</v>
-      </c>
-      <c r="X87" t="s">
-        <v>457</v>
-      </c>
-      <c r="Y87" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B88">
         <v>12505779</v>
@@ -9177,21 +9177,21 @@
         <v>38</v>
       </c>
       <c r="V88" t="s">
+        <v>461</v>
+      </c>
+      <c r="W88" t="s">
         <v>462</v>
-      </c>
-      <c r="W88" t="s">
-        <v>463</v>
       </c>
       <c r="X88" t="s">
         <v>48</v>
       </c>
       <c r="Y88" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B89">
         <v>12505772</v>
@@ -9218,7 +9218,7 @@
         <v>314</v>
       </c>
       <c r="J89" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K89"/>
       <c r="L89" t="s">
@@ -9230,7 +9230,7 @@
       <c r="N89"/>
       <c r="O89"/>
       <c r="P89" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Q89">
         <v>581.5</v>
@@ -9248,21 +9248,21 @@
         <v>38</v>
       </c>
       <c r="V89" t="s">
+        <v>467</v>
+      </c>
+      <c r="W89" t="s">
         <v>468</v>
-      </c>
-      <c r="W89" t="s">
-        <v>469</v>
       </c>
       <c r="X89" t="s">
         <v>314</v>
       </c>
       <c r="Y89" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B90">
         <v>12505771</v>
@@ -9289,7 +9289,7 @@
         <v>175</v>
       </c>
       <c r="J90" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K90"/>
       <c r="L90" t="s">
@@ -9301,7 +9301,7 @@
       <c r="N90"/>
       <c r="O90"/>
       <c r="P90" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q90">
         <v>581.5</v>
@@ -9319,24 +9319,24 @@
         <v>38</v>
       </c>
       <c r="V90" t="s">
+        <v>472</v>
+      </c>
+      <c r="W90" t="s">
         <v>473</v>
-      </c>
-      <c r="W90" t="s">
-        <v>474</v>
       </c>
       <c r="X90" t="s">
         <v>175</v>
       </c>
       <c r="Y90" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>475</v>
+      </c>
+      <c r="B91" t="s">
         <v>476</v>
-      </c>
-      <c r="B91" t="s">
-        <v>477</v>
       </c>
       <c r="C91" t="s">
         <v>194</v>
@@ -9373,10 +9373,10 @@
         <v>59</v>
       </c>
       <c r="O91" t="s">
+        <v>477</v>
+      </c>
+      <c r="P91" t="s">
         <v>478</v>
-      </c>
-      <c r="P91" t="s">
-        <v>479</v>
       </c>
       <c r="Q91">
         <v>698.03</v>
@@ -9394,24 +9394,24 @@
         <v>38</v>
       </c>
       <c r="V91" t="s">
+        <v>479</v>
+      </c>
+      <c r="W91" t="s">
         <v>480</v>
-      </c>
-      <c r="W91" t="s">
-        <v>481</v>
       </c>
       <c r="X91" t="s">
         <v>63</v>
       </c>
       <c r="Y91" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>482</v>
+      </c>
+      <c r="B92" t="s">
         <v>483</v>
-      </c>
-      <c r="B92" t="s">
-        <v>484</v>
       </c>
       <c r="C92" t="s">
         <v>194</v>
@@ -9451,7 +9451,7 @@
         <v>401</v>
       </c>
       <c r="P92" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q92">
         <v>756.12</v>
@@ -9469,24 +9469,24 @@
         <v>38</v>
       </c>
       <c r="V92" t="s">
+        <v>484</v>
+      </c>
+      <c r="W92" t="s">
         <v>485</v>
-      </c>
-      <c r="W92" t="s">
-        <v>486</v>
       </c>
       <c r="X92" t="s">
         <v>314</v>
       </c>
       <c r="Y92" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>487</v>
+      </c>
+      <c r="B93" t="s">
         <v>488</v>
-      </c>
-      <c r="B93" t="s">
-        <v>489</v>
       </c>
       <c r="C93" t="s">
         <v>194</v>
@@ -9526,7 +9526,7 @@
         <v>60</v>
       </c>
       <c r="P93" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q93">
         <v>756.12</v>
@@ -9544,24 +9544,24 @@
         <v>38</v>
       </c>
       <c r="V93" t="s">
+        <v>489</v>
+      </c>
+      <c r="W93" t="s">
         <v>490</v>
-      </c>
-      <c r="W93" t="s">
-        <v>491</v>
       </c>
       <c r="X93" t="s">
         <v>48</v>
       </c>
       <c r="Y93" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>492</v>
+      </c>
+      <c r="B94" t="s">
         <v>493</v>
-      </c>
-      <c r="B94" t="s">
-        <v>494</v>
       </c>
       <c r="C94" t="s">
         <v>194</v>
@@ -9601,7 +9601,7 @@
         <v>60</v>
       </c>
       <c r="P94" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q94">
         <v>756.12</v>
@@ -9619,24 +9619,24 @@
         <v>38</v>
       </c>
       <c r="V94" t="s">
+        <v>494</v>
+      </c>
+      <c r="W94" t="s">
         <v>495</v>
-      </c>
-      <c r="W94" t="s">
-        <v>496</v>
       </c>
       <c r="X94" t="s">
         <v>41</v>
       </c>
       <c r="Y94" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>497</v>
+      </c>
+      <c r="B95" t="s">
         <v>498</v>
-      </c>
-      <c r="B95" t="s">
-        <v>499</v>
       </c>
       <c r="C95" t="s">
         <v>194</v>
@@ -9673,10 +9673,10 @@
         <v>59</v>
       </c>
       <c r="O95" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="P95" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q95">
         <v>581.5</v>
@@ -9694,21 +9694,21 @@
         <v>38</v>
       </c>
       <c r="V95" t="s">
+        <v>500</v>
+      </c>
+      <c r="W95" t="s">
         <v>501</v>
-      </c>
-      <c r="W95" t="s">
-        <v>502</v>
       </c>
       <c r="X95" t="s">
         <v>41</v>
       </c>
       <c r="Y95" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B96">
         <v>12489441</v>
@@ -9747,7 +9747,7 @@
       <c r="N96"/>
       <c r="O96"/>
       <c r="P96" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q96">
         <v>581.5</v>
@@ -9765,21 +9765,21 @@
         <v>38</v>
       </c>
       <c r="V96" t="s">
+        <v>504</v>
+      </c>
+      <c r="W96" t="s">
         <v>505</v>
-      </c>
-      <c r="W96" t="s">
-        <v>506</v>
       </c>
       <c r="X96" t="s">
         <v>76</v>
       </c>
       <c r="Y96" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B97">
         <v>12489435</v>
@@ -9800,7 +9800,7 @@
         <v>29</v>
       </c>
       <c r="H97" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I97" t="s">
         <v>314</v>
@@ -9818,7 +9818,7 @@
       <c r="N97"/>
       <c r="O97"/>
       <c r="P97" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q97">
         <v>558.33000000000004</v>
@@ -9836,21 +9836,21 @@
         <v>38</v>
       </c>
       <c r="V97" t="s">
+        <v>510</v>
+      </c>
+      <c r="W97" t="s">
         <v>511</v>
-      </c>
-      <c r="W97" t="s">
-        <v>512</v>
       </c>
       <c r="X97" t="s">
         <v>314</v>
       </c>
       <c r="Y97" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B98">
         <v>12489434</v>
@@ -9871,7 +9871,7 @@
         <v>29</v>
       </c>
       <c r="H98" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I98" t="s">
         <v>415</v>
@@ -9889,7 +9889,7 @@
       <c r="N98"/>
       <c r="O98"/>
       <c r="P98" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q98">
         <v>744.59</v>
@@ -9907,21 +9907,21 @@
         <v>38</v>
       </c>
       <c r="V98" t="s">
+        <v>515</v>
+      </c>
+      <c r="W98" t="s">
         <v>516</v>
-      </c>
-      <c r="W98" t="s">
-        <v>517</v>
       </c>
       <c r="X98" t="s">
         <v>63</v>
       </c>
       <c r="Y98" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B99">
         <v>12309046</v>
@@ -9942,10 +9942,10 @@
         <v>29</v>
       </c>
       <c r="H99" t="s">
+        <v>519</v>
+      </c>
+      <c r="I99" t="s">
         <v>520</v>
-      </c>
-      <c r="I99" t="s">
-        <v>521</v>
       </c>
       <c r="J99" t="s">
         <v>32</v>
@@ -9962,7 +9962,7 @@
       <c r="N99"/>
       <c r="O99"/>
       <c r="P99" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="Q99">
         <v>997.4</v>
@@ -9980,24 +9980,24 @@
         <v>38</v>
       </c>
       <c r="V99" t="s">
+        <v>522</v>
+      </c>
+      <c r="W99" t="s">
         <v>523</v>
-      </c>
-      <c r="W99" t="s">
-        <v>524</v>
       </c>
       <c r="X99" t="s">
         <v>148</v>
       </c>
       <c r="Y99" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>525</v>
+      </c>
+      <c r="B100" t="s">
         <v>526</v>
-      </c>
-      <c r="B100" t="s">
-        <v>527</v>
       </c>
       <c r="C100" t="s">
         <v>45</v>
@@ -10039,7 +10039,7 @@
         <v>69</v>
       </c>
       <c r="P100" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q100">
         <v>1210.25</v>
@@ -10057,24 +10057,24 @@
         <v>38</v>
       </c>
       <c r="V100" t="s">
+        <v>528</v>
+      </c>
+      <c r="W100" t="s">
         <v>529</v>
-      </c>
-      <c r="W100" t="s">
-        <v>530</v>
       </c>
       <c r="X100" t="s">
         <v>48</v>
       </c>
       <c r="Y100" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>531</v>
+      </c>
+      <c r="B101" t="s">
         <v>532</v>
-      </c>
-      <c r="B101" t="s">
-        <v>533</v>
       </c>
       <c r="C101" t="s">
         <v>45</v>
@@ -10116,7 +10116,7 @@
         <v>86</v>
       </c>
       <c r="P101" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q101">
         <v>1210.25</v>
@@ -10134,24 +10134,24 @@
         <v>38</v>
       </c>
       <c r="V101" t="s">
+        <v>533</v>
+      </c>
+      <c r="W101" t="s">
         <v>534</v>
-      </c>
-      <c r="W101" t="s">
-        <v>535</v>
       </c>
       <c r="X101" t="s">
         <v>48</v>
       </c>
       <c r="Y101" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>536</v>
+      </c>
+      <c r="B102" t="s">
         <v>537</v>
-      </c>
-      <c r="B102" t="s">
-        <v>538</v>
       </c>
       <c r="C102" t="s">
         <v>45</v>
@@ -10193,7 +10193,7 @@
         <v>69</v>
       </c>
       <c r="P102" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Q102">
         <v>1769.05</v>
@@ -10211,21 +10211,21 @@
         <v>38</v>
       </c>
       <c r="V102" t="s">
+        <v>539</v>
+      </c>
+      <c r="W102" t="s">
         <v>540</v>
-      </c>
-      <c r="W102" t="s">
-        <v>541</v>
       </c>
       <c r="X102" t="s">
         <v>48</v>
       </c>
       <c r="Y102" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B103">
         <v>12162668</v>
@@ -10266,7 +10266,7 @@
       <c r="N103"/>
       <c r="O103"/>
       <c r="P103" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="Q103">
         <v>791.16</v>
@@ -10284,24 +10284,24 @@
         <v>38</v>
       </c>
       <c r="V103" t="s">
+        <v>543</v>
+      </c>
+      <c r="W103" t="s">
         <v>544</v>
-      </c>
-      <c r="W103" t="s">
-        <v>545</v>
       </c>
       <c r="X103" t="s">
         <v>48</v>
       </c>
       <c r="Y103" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>546</v>
+      </c>
+      <c r="B104" t="s">
         <v>547</v>
-      </c>
-      <c r="B104" t="s">
-        <v>548</v>
       </c>
       <c r="C104" t="s">
         <v>194</v>
@@ -10341,7 +10341,7 @@
         <v>69</v>
       </c>
       <c r="P104" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Q104">
         <v>1396.52</v>
@@ -10359,24 +10359,24 @@
         <v>38</v>
       </c>
       <c r="V104" t="s">
+        <v>549</v>
+      </c>
+      <c r="W104" t="s">
         <v>550</v>
-      </c>
-      <c r="W104" t="s">
-        <v>551</v>
       </c>
       <c r="X104" t="s">
         <v>48</v>
       </c>
       <c r="Y104" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>552</v>
+      </c>
+      <c r="B105" t="s">
         <v>553</v>
-      </c>
-      <c r="B105" t="s">
-        <v>554</v>
       </c>
       <c r="C105" t="s">
         <v>194</v>
@@ -10394,7 +10394,7 @@
         <v>29</v>
       </c>
       <c r="H105" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I105" t="s">
         <v>48</v>
@@ -10416,7 +10416,7 @@
         <v>60</v>
       </c>
       <c r="P105" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Q105">
         <v>1396.52</v>
@@ -10434,24 +10434,24 @@
         <v>38</v>
       </c>
       <c r="V105" t="s">
+        <v>555</v>
+      </c>
+      <c r="W105" t="s">
         <v>556</v>
-      </c>
-      <c r="W105" t="s">
-        <v>557</v>
       </c>
       <c r="X105" t="s">
         <v>48</v>
       </c>
       <c r="Y105" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>558</v>
+      </c>
+      <c r="B106" t="s">
         <v>559</v>
-      </c>
-      <c r="B106" t="s">
-        <v>560</v>
       </c>
       <c r="C106" t="s">
         <v>194</v>
@@ -10469,7 +10469,7 @@
         <v>29</v>
       </c>
       <c r="H106" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I106" t="s">
         <v>41</v>
@@ -10491,7 +10491,7 @@
         <v>401</v>
       </c>
       <c r="P106" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q106">
         <v>581.5</v>
@@ -10509,21 +10509,21 @@
         <v>38</v>
       </c>
       <c r="V106" t="s">
+        <v>561</v>
+      </c>
+      <c r="W106" t="s">
         <v>562</v>
-      </c>
-      <c r="W106" t="s">
-        <v>563</v>
       </c>
       <c r="X106" t="s">
         <v>41</v>
       </c>
       <c r="Y106" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B107">
         <v>12033128</v>
@@ -10562,7 +10562,7 @@
       <c r="N107"/>
       <c r="O107"/>
       <c r="P107" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="Q107">
         <v>750.95</v>
@@ -10580,21 +10580,21 @@
         <v>38</v>
       </c>
       <c r="V107" t="s">
+        <v>566</v>
+      </c>
+      <c r="W107" t="s">
         <v>567</v>
-      </c>
-      <c r="W107" t="s">
-        <v>568</v>
       </c>
       <c r="X107" t="s">
         <v>48</v>
       </c>
       <c r="Y107" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B108">
         <v>12033103</v>
@@ -10633,7 +10633,7 @@
       <c r="N108"/>
       <c r="O108"/>
       <c r="P108" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q108">
         <v>581.5</v>
@@ -10651,21 +10651,21 @@
         <v>38</v>
       </c>
       <c r="V108" t="s">
+        <v>570</v>
+      </c>
+      <c r="W108" t="s">
         <v>571</v>
-      </c>
-      <c r="W108" t="s">
-        <v>572</v>
       </c>
       <c r="X108" t="s">
         <v>48</v>
       </c>
       <c r="Y108" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B109">
         <v>12033099</v>
@@ -10704,7 +10704,7 @@
       <c r="N109"/>
       <c r="O109"/>
       <c r="P109" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="Q109">
         <v>581.5</v>
@@ -10722,21 +10722,21 @@
         <v>38</v>
       </c>
       <c r="V109" t="s">
+        <v>575</v>
+      </c>
+      <c r="W109" t="s">
         <v>576</v>
-      </c>
-      <c r="W109" t="s">
-        <v>577</v>
       </c>
       <c r="X109" t="s">
         <v>175</v>
       </c>
       <c r="Y109" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B110">
         <v>12033078</v>
@@ -10775,7 +10775,7 @@
       <c r="N110"/>
       <c r="O110"/>
       <c r="P110" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q110">
         <v>744.59</v>
@@ -10793,21 +10793,21 @@
         <v>38</v>
       </c>
       <c r="V110" t="s">
+        <v>579</v>
+      </c>
+      <c r="W110" t="s">
         <v>580</v>
-      </c>
-      <c r="W110" t="s">
-        <v>581</v>
       </c>
       <c r="X110" t="s">
         <v>48</v>
       </c>
       <c r="Y110" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B111">
         <v>12033074</v>
@@ -10828,7 +10828,7 @@
         <v>29</v>
       </c>
       <c r="H111" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I111" t="s">
         <v>138</v>
@@ -10846,7 +10846,7 @@
       <c r="N111"/>
       <c r="O111"/>
       <c r="P111" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q111">
         <v>744.59</v>
@@ -10864,21 +10864,21 @@
         <v>38</v>
       </c>
       <c r="V111" t="s">
+        <v>584</v>
+      </c>
+      <c r="W111" t="s">
         <v>585</v>
-      </c>
-      <c r="W111" t="s">
-        <v>586</v>
       </c>
       <c r="X111" t="s">
         <v>41</v>
       </c>
       <c r="Y111" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B112">
         <v>11601067</v>
@@ -10899,7 +10899,7 @@
         <v>29</v>
       </c>
       <c r="H112" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I112" t="s">
         <v>41</v>
@@ -10917,7 +10917,7 @@
       <c r="N112"/>
       <c r="O112"/>
       <c r="P112" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="Q112">
         <v>465.2</v>
@@ -10935,21 +10935,21 @@
         <v>38</v>
       </c>
       <c r="V112" t="s">
+        <v>589</v>
+      </c>
+      <c r="W112" t="s">
         <v>590</v>
-      </c>
-      <c r="W112" t="s">
-        <v>591</v>
       </c>
       <c r="X112" t="s">
         <v>41</v>
       </c>
       <c r="Y112" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B113">
         <v>11601006</v>
@@ -10970,10 +10970,10 @@
         <v>29</v>
       </c>
       <c r="H113" t="s">
+        <v>593</v>
+      </c>
+      <c r="I113" t="s">
         <v>594</v>
-      </c>
-      <c r="I113" t="s">
-        <v>595</v>
       </c>
       <c r="J113" t="s">
         <v>197</v>
@@ -11006,21 +11006,21 @@
         <v>38</v>
       </c>
       <c r="V113" t="s">
+        <v>595</v>
+      </c>
+      <c r="W113" t="s">
         <v>596</v>
-      </c>
-      <c r="W113" t="s">
-        <v>597</v>
       </c>
       <c r="X113" t="s">
         <v>41</v>
       </c>
       <c r="Y113" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B114">
         <v>11600974</v>
@@ -11041,7 +11041,7 @@
         <v>29</v>
       </c>
       <c r="H114" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I114" t="s">
         <v>63</v>
@@ -11077,24 +11077,24 @@
         <v>38</v>
       </c>
       <c r="V114" t="s">
+        <v>600</v>
+      </c>
+      <c r="W114" t="s">
         <v>601</v>
-      </c>
-      <c r="W114" t="s">
-        <v>602</v>
       </c>
       <c r="X114" t="s">
         <v>63</v>
       </c>
       <c r="Y114" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>603</v>
+      </c>
+      <c r="B115" t="s">
         <v>604</v>
-      </c>
-      <c r="B115" t="s">
-        <v>605</v>
       </c>
       <c r="C115" t="s">
         <v>194</v>
@@ -11131,10 +11131,10 @@
         <v>392</v>
       </c>
       <c r="O115" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="P115" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q115">
         <v>581.5</v>
@@ -11152,24 +11152,24 @@
         <v>38</v>
       </c>
       <c r="V115" t="s">
+        <v>606</v>
+      </c>
+      <c r="W115" t="s">
         <v>607</v>
-      </c>
-      <c r="W115" t="s">
-        <v>608</v>
       </c>
       <c r="X115" t="s">
         <v>41</v>
       </c>
       <c r="Y115" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>609</v>
+      </c>
+      <c r="B116" t="s">
         <v>610</v>
-      </c>
-      <c r="B116" t="s">
-        <v>611</v>
       </c>
       <c r="C116" t="s">
         <v>194</v>
@@ -11190,7 +11190,7 @@
         <v>408</v>
       </c>
       <c r="I116" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J116" t="s">
         <v>197</v>
@@ -11209,7 +11209,7 @@
         <v>401</v>
       </c>
       <c r="P116" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q116">
         <v>756.12</v>
@@ -11227,24 +11227,24 @@
         <v>38</v>
       </c>
       <c r="V116" t="s">
+        <v>612</v>
+      </c>
+      <c r="W116" t="s">
         <v>613</v>
-      </c>
-      <c r="W116" t="s">
-        <v>614</v>
       </c>
       <c r="X116" t="s">
         <v>63</v>
       </c>
       <c r="Y116" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>615</v>
+      </c>
+      <c r="B117" t="s">
         <v>616</v>
-      </c>
-      <c r="B117" t="s">
-        <v>617</v>
       </c>
       <c r="C117" t="s">
         <v>194</v>
@@ -11265,7 +11265,7 @@
         <v>408</v>
       </c>
       <c r="I117" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J117" t="s">
         <v>197</v>
@@ -11284,7 +11284,7 @@
         <v>60</v>
       </c>
       <c r="P117" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q117">
         <v>756.12</v>
@@ -11302,24 +11302,24 @@
         <v>38</v>
       </c>
       <c r="V117" t="s">
+        <v>618</v>
+      </c>
+      <c r="W117" t="s">
         <v>619</v>
-      </c>
-      <c r="W117" t="s">
-        <v>620</v>
       </c>
       <c r="X117" t="s">
         <v>63</v>
       </c>
       <c r="Y117" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>621</v>
+      </c>
+      <c r="B118" t="s">
         <v>622</v>
-      </c>
-      <c r="B118" t="s">
-        <v>623</v>
       </c>
       <c r="C118" t="s">
         <v>45</v>
@@ -11361,7 +11361,7 @@
         <v>401</v>
       </c>
       <c r="P118" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="Q118">
         <v>750.95</v>
@@ -11379,21 +11379,21 @@
         <v>38</v>
       </c>
       <c r="V118" t="s">
+        <v>624</v>
+      </c>
+      <c r="W118" t="s">
         <v>625</v>
-      </c>
-      <c r="W118" t="s">
-        <v>626</v>
       </c>
       <c r="X118" t="s">
         <v>168</v>
       </c>
       <c r="Y118" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B119">
         <v>11277642</v>
@@ -11414,10 +11414,10 @@
         <v>29</v>
       </c>
       <c r="H119" t="s">
+        <v>628</v>
+      </c>
+      <c r="I119" t="s">
         <v>629</v>
-      </c>
-      <c r="I119" t="s">
-        <v>630</v>
       </c>
       <c r="J119" t="s">
         <v>197</v>
@@ -11450,21 +11450,21 @@
         <v>38</v>
       </c>
       <c r="V119" t="s">
+        <v>630</v>
+      </c>
+      <c r="W119" t="s">
         <v>631</v>
-      </c>
-      <c r="W119" t="s">
-        <v>632</v>
       </c>
       <c r="X119" t="s">
         <v>41</v>
       </c>
       <c r="Y119" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B120">
         <v>11179873</v>
@@ -11485,13 +11485,13 @@
         <v>29</v>
       </c>
       <c r="H120" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I120" t="s">
         <v>63</v>
       </c>
       <c r="J120" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="K120"/>
       <c r="L120" t="s">
@@ -11503,7 +11503,7 @@
       <c r="N120"/>
       <c r="O120"/>
       <c r="P120" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q120">
         <v>1117.1199999999999</v>
@@ -11521,21 +11521,21 @@
         <v>38</v>
       </c>
       <c r="V120" t="s">
+        <v>636</v>
+      </c>
+      <c r="W120" t="s">
         <v>637</v>
-      </c>
-      <c r="W120" t="s">
-        <v>638</v>
       </c>
       <c r="X120" t="s">
         <v>63</v>
       </c>
       <c r="Y120" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B121">
         <v>11179873</v>
@@ -11556,13 +11556,13 @@
         <v>29</v>
       </c>
       <c r="H121" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I121" t="s">
         <v>63</v>
       </c>
       <c r="J121" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="K121"/>
       <c r="L121" t="s">
@@ -11574,7 +11574,7 @@
       <c r="N121"/>
       <c r="O121"/>
       <c r="P121" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q121">
         <v>1117.1199999999999</v>
@@ -11592,21 +11592,21 @@
         <v>38</v>
       </c>
       <c r="V121" t="s">
+        <v>636</v>
+      </c>
+      <c r="W121" t="s">
         <v>637</v>
-      </c>
-      <c r="W121" t="s">
-        <v>638</v>
       </c>
       <c r="X121" t="s">
         <v>63</v>
       </c>
       <c r="Y121" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B122">
         <v>11179866</v>
@@ -11627,7 +11627,7 @@
         <v>29</v>
       </c>
       <c r="H122" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I122" t="s">
         <v>48</v>
@@ -11647,7 +11647,7 @@
       <c r="N122"/>
       <c r="O122"/>
       <c r="P122" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q122">
         <v>1163.57</v>
@@ -11665,21 +11665,21 @@
         <v>38</v>
       </c>
       <c r="V122" t="s">
+        <v>642</v>
+      </c>
+      <c r="W122" t="s">
         <v>643</v>
-      </c>
-      <c r="W122" t="s">
-        <v>644</v>
       </c>
       <c r="X122" t="s">
         <v>48</v>
       </c>
       <c r="Y122" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B123">
         <v>11179834</v>
@@ -11700,7 +11700,7 @@
         <v>29</v>
       </c>
       <c r="H123" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I123" t="s">
         <v>63</v>
@@ -11720,7 +11720,7 @@
       <c r="N123"/>
       <c r="O123"/>
       <c r="P123" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q123">
         <v>1163.57</v>
@@ -11738,21 +11738,21 @@
         <v>38</v>
       </c>
       <c r="V123" t="s">
+        <v>647</v>
+      </c>
+      <c r="W123" t="s">
         <v>648</v>
-      </c>
-      <c r="W123" t="s">
-        <v>649</v>
       </c>
       <c r="X123" t="s">
         <v>63</v>
       </c>
       <c r="Y123" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B124">
         <v>11179831</v>
@@ -11793,7 +11793,7 @@
       <c r="N124"/>
       <c r="O124"/>
       <c r="P124" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q124">
         <v>1163.57</v>
@@ -11811,24 +11811,24 @@
         <v>38</v>
       </c>
       <c r="V124" t="s">
+        <v>651</v>
+      </c>
+      <c r="W124" t="s">
         <v>652</v>
-      </c>
-      <c r="W124" t="s">
-        <v>653</v>
       </c>
       <c r="X124" t="s">
         <v>48</v>
       </c>
       <c r="Y124" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>654</v>
+      </c>
+      <c r="B125" t="s">
         <v>655</v>
-      </c>
-      <c r="B125" t="s">
-        <v>656</v>
       </c>
       <c r="C125" t="s">
         <v>45</v>
@@ -11846,7 +11846,7 @@
         <v>29</v>
       </c>
       <c r="H125" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I125" t="s">
         <v>48</v>
@@ -11870,7 +11870,7 @@
         <v>60</v>
       </c>
       <c r="P125" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="Q125">
         <v>1489.65</v>
@@ -11888,24 +11888,24 @@
         <v>38</v>
       </c>
       <c r="V125" t="s">
+        <v>657</v>
+      </c>
+      <c r="W125" t="s">
         <v>658</v>
-      </c>
-      <c r="W125" t="s">
-        <v>659</v>
       </c>
       <c r="X125" t="s">
         <v>48</v>
       </c>
       <c r="Y125" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>660</v>
+      </c>
+      <c r="B126" t="s">
         <v>661</v>
-      </c>
-      <c r="B126" t="s">
-        <v>662</v>
       </c>
       <c r="C126" t="s">
         <v>45</v>
@@ -11926,7 +11926,7 @@
         <v>47</v>
       </c>
       <c r="I126" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J126" t="s">
         <v>125</v>
@@ -11963,24 +11963,24 @@
         <v>38</v>
       </c>
       <c r="V126" t="s">
+        <v>663</v>
+      </c>
+      <c r="W126" t="s">
         <v>664</v>
-      </c>
-      <c r="W126" t="s">
-        <v>665</v>
       </c>
       <c r="X126" t="s">
         <v>48</v>
       </c>
       <c r="Y126" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>666</v>
+      </c>
+      <c r="B127" t="s">
         <v>667</v>
-      </c>
-      <c r="B127" t="s">
-        <v>668</v>
       </c>
       <c r="C127" t="s">
         <v>45</v>
@@ -11998,10 +11998,10 @@
         <v>29</v>
       </c>
       <c r="H127" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I127" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J127" t="s">
         <v>125</v>
@@ -12038,16 +12038,16 @@
         <v>38</v>
       </c>
       <c r="V127" t="s">
+        <v>669</v>
+      </c>
+      <c r="W127" t="s">
         <v>670</v>
-      </c>
-      <c r="W127" t="s">
-        <v>671</v>
       </c>
       <c r="X127" t="s">
         <v>63</v>
       </c>
       <c r="Y127" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>